<commit_message>
fix mock input files, add fixture and test_init
</commit_message>
<xml_diff>
--- a/EchoPro/test_data/input_files/Stratification/Stratification_geographic_Lat_final.xlsx
+++ b/EchoPro/test_data/input_files/Stratification/Stratification_geographic_Lat_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wujung/code_git/EchoPro/EchoPro/test_data/input_files/Stratification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4206F2AD-700B-F143-A9B2-8DDF37C17322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C183963F-72F7-EC4B-A6CF-ECAA52B3C0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
-  <si>
-    <t>Latitude (upper limit)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>haul start</t>
   </si>
@@ -370,26 +367,26 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -406,7 +403,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -426,19 +423,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -455,7 +452,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>